<commit_message>
Add 500 ms graph
</commit_message>
<xml_diff>
--- a/Assignment 3/Diagrams.xlsx
+++ b/Assignment 3/Diagrams.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\assignment-di-reti\Assignment 3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0285DCA9-61BF-4415-895E-B1D622EAE668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -20,41 +31,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
-    <t xml:space="preserve">--------------------</t>
+    <t>--------------------</t>
   </si>
   <si>
-    <t xml:space="preserve">SERVER_DELAY 0 ms</t>
+    <t>SERVER_DELAY 0 ms</t>
   </si>
   <si>
-    <t xml:space="preserve">PAYLOAD</t>
+    <t>PAYLOAD</t>
   </si>
   <si>
-    <t xml:space="preserve">RTT</t>
+    <t>RTT</t>
   </si>
   <si>
-    <t xml:space="preserve">THPUT</t>
+    <t>THPUT</t>
   </si>
   <si>
-    <t xml:space="preserve">SERVER_DELAY 10 ms</t>
+    <t>SERVER_DELAY 10 ms</t>
   </si>
   <si>
-    <t xml:space="preserve">SERVER_DELAY 50 ms</t>
+    <t>SERVER_DELAY 50 ms</t>
+  </si>
+  <si>
+    <t>SERVER_DELAY 500 ms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -63,22 +75,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -86,30 +83,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <strike val="true"/>
+      <strike/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,7 +100,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -129,69 +108,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -250,15 +183,33 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -267,7 +218,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -275,7 +226,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -296,6 +247,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -314,12 +266,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472c4"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -329,24 +278,31 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -355,13 +311,20 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Foglio1!$D$5:$I$5</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -381,20 +344,20 @@
                 <c:pt idx="5">
                   <c:v>1000</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Foglio1!$D$6:$I$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.09145</c:v>
+                  <c:v>9.1450000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1059</c:v>
+                  <c:v>0.10589999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.10865</c:v>
@@ -403,16 +366,29 @@
                   <c:v>0.11475</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11535</c:v>
+                  <c:v>0.11534999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1165</c:v>
+                  <c:v>0.11650000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F738-4674-B7C1-90C7080D2F96}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -421,6 +397,7 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="57917352"/>
         <c:axId val="14506580"/>
       </c:lineChart>
@@ -438,7 +415,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -446,7 +423,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -472,7 +449,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -482,13 +459,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="14506580"/>
@@ -496,6 +474,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="14506580"/>
@@ -508,7 +487,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -521,7 +500,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -529,7 +508,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -562,13 +541,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="57917352"/>
@@ -584,25 +564,33 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -611,7 +599,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -619,7 +607,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -640,6 +628,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -658,12 +647,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472c4"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -673,24 +659,31 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.000" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -699,13 +692,20 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Foglio1!$D$8:$H$8</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
@@ -722,35 +722,48 @@
                 <c:pt idx="4">
                   <c:v>32000</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Foglio1!$D$9:$H$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>66567.41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>88394.382</c:v>
+                  <c:v>88394.381999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>127427.437</c:v>
+                  <c:v>127427.43700000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>454635.218</c:v>
+                  <c:v>454635.21799999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>843234.062</c:v>
+                  <c:v>843234.06200000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-54B8-4D58-83E3-863940FD1EF2}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -759,6 +772,7 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="28563300"/>
         <c:axId val="20377141"/>
       </c:lineChart>
@@ -776,7 +790,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -784,7 +798,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -810,7 +824,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -820,13 +834,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="20377141"/>
@@ -834,6 +849,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="20377141"/>
@@ -846,7 +862,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -859,7 +875,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -867,7 +883,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -900,13 +916,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="28563300"/>
@@ -922,25 +939,33 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -949,7 +974,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -957,7 +982,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -978,6 +1003,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -996,12 +1022,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472c4"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1011,24 +1034,31 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0.000000" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1037,13 +1067,20 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Foglio1!$D$32:$I$32</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -1063,20 +1100,20 @@
                 <c:pt idx="5">
                   <c:v>1000</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Foglio1!$D$33:$I$33</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>10.507</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.614</c:v>
+                  <c:v>10.614000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10.5945</c:v>
@@ -1088,13 +1125,26 @@
                   <c:v>10.7037</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.8234</c:v>
+                  <c:v>10.823399999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8645-48E9-9B3A-9389F7C19815}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -1103,6 +1153,7 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="59119462"/>
         <c:axId val="71557302"/>
       </c:lineChart>
@@ -1120,7 +1171,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1128,7 +1179,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1154,7 +1205,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1164,13 +1215,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="71557302"/>
@@ -1178,6 +1230,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="71557302"/>
@@ -1190,7 +1243,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1203,7 +1256,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1211,7 +1264,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1244,13 +1297,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="59119462"/>
@@ -1266,25 +1320,33 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1293,7 +1355,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1301,7 +1363,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1322,6 +1384,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1340,12 +1403,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472c4"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1355,24 +1415,31 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.000" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1381,13 +1448,20 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Foglio1!$D$35:$H$35</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
@@ -1404,14 +1478,14 @@
                 <c:pt idx="4">
                   <c:v>32000</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Foglio1!$D$36:$H$36</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>737.39</c:v>
@@ -1423,7 +1497,7 @@
                   <c:v>2999.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11512.933</c:v>
+                  <c:v>11512.933000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>23858.7</c:v>
@@ -1432,7 +1506,20 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-212D-4BAD-8A0B-74651098D605}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -1441,6 +1528,7 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="22102846"/>
         <c:axId val="51360146"/>
       </c:lineChart>
@@ -1458,7 +1546,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1466,7 +1554,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1492,7 +1580,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1502,13 +1590,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="51360146"/>
@@ -1516,6 +1605,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="51360146"/>
@@ -1528,7 +1618,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1541,7 +1631,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1549,7 +1639,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1564,8 +1654,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0279103053435115"/>
-              <c:y val="0.809817561359758"/>
+              <c:x val="2.79103053435115E-2"/>
+              <c:y val="0.80981756135975802"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1590,13 +1680,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="22102846"/>
@@ -1612,25 +1703,33 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1639,7 +1738,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1647,7 +1746,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1668,6 +1767,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1686,12 +1786,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472c4"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1701,24 +1798,31 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0.000000" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1727,13 +1831,20 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Foglio1!$D$60:$I$60</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -1753,29 +1864,29 @@
                 <c:pt idx="5">
                   <c:v>1000</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Foglio1!$D$61:$I$61</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0.000000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>50.664249</c:v>
+                  <c:v>50.664248999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.6443</c:v>
+                  <c:v>50.644300000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.7387</c:v>
+                  <c:v>50.738700000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.7908</c:v>
+                  <c:v>50.790799999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.7981</c:v>
+                  <c:v>50.798099999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>50.9861</c:v>
@@ -1784,7 +1895,20 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F25C-4F09-AC97-44C615C1297F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -1793,6 +1917,7 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="31087761"/>
         <c:axId val="57253416"/>
       </c:lineChart>
@@ -1810,7 +1935,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1818,7 +1943,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1844,7 +1969,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1854,13 +1979,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="57253416"/>
@@ -1868,6 +1994,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="57253416"/>
@@ -1880,7 +2007,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1893,7 +2020,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1901,7 +2028,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -1934,13 +2061,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="31087761"/>
@@ -1956,25 +2084,33 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1983,7 +2119,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1991,7 +2127,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
+              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -2012,6 +2148,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -2030,12 +2167,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472c4"/>
-            </a:solidFill>
             <a:ln w="28440">
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2045,24 +2179,31 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="0.000" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -2071,13 +2212,20 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Foglio1!$D$63:$H$63</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
@@ -2094,35 +2242,48 @@
                 <c:pt idx="4">
                   <c:v>32000</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Foglio1!$D$64:$H$64</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>157.98</c:v>
+                  <c:v>157.97999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>312.8258</c:v>
+                  <c:v>312.82580000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>620.9144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2503.5878</c:v>
+                  <c:v>2503.5877999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5056.864</c:v>
+                  <c:v>5056.8639999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3428-4C87-9AE1-BED52D2D4836}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln>
@@ -2131,6 +2292,7 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="7713162"/>
         <c:axId val="86428279"/>
       </c:lineChart>
@@ -2148,7 +2310,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2156,7 +2318,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2182,7 +2344,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -2192,13 +2354,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="86428279"/>
@@ -2206,6 +2369,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="86428279"/>
@@ -2218,7 +2382,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2231,7 +2395,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2239,7 +2403,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -2272,13 +2436,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="7713162"/>
@@ -2294,23 +2459,799 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>RTT con delay di 500 ms</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$C$89</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RTT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="4472C4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4472C4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Foglio1!$D$88:$I$88</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$D$89:$I$89</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.000000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>500.667419</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.67169200000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500.66989999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500.72390000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500.87279999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500.91579999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9865-4F80-A22F-CFB61984AF56}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="31087761"/>
+        <c:axId val="57253416"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="31087761"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>PAYLOAD (Byte)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="D9D9D9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="57253416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="57253416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>RTT (Millisecondi)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="31087761"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="D9D9D9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>THROUGHPUT con delay di 500 ms</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Foglio1!$C$92</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>THPUT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28440">
+              <a:solidFill>
+                <a:srgbClr val="4472C4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4472C4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Foglio1!$D$91:$H$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$D$92:$H$92</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16.0732</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.031199999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.948999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>255.43940000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>510.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E855-4E75-BF45-A11A520CB7B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="7713162"/>
+        <c:axId val="86428279"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="7713162"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>PAYLOAD (Byte)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="D9D9D9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="86428279"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="86428279"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>THROUGHPUT (Kilobit/Secondo)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7713162"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="D9D9D9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2320,18 +3261,24 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>608040</xdr:colOff>
+      <xdr:colOff>209455</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Grafico 15"/>
+        <xdr:cNvPr id="2" name="Grafico 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="781560" y="2017080"/>
-        <a:ext cx="4778640" cy="2742480"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2350,18 +3297,24 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>340200</xdr:colOff>
+      <xdr:colOff>340201</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Grafico 16"/>
+        <xdr:cNvPr id="3" name="Grafico 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6378480" y="2011680"/>
-        <a:ext cx="4746240" cy="2733480"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2379,19 +3332,25 @@
       <xdr:rowOff>11520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>319320</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>712043</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>10800</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafico 17"/>
+        <xdr:cNvPr id="4" name="Grafico 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="611280" y="6869520"/>
-        <a:ext cx="4660200" cy="2742480"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2410,18 +3369,24 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>327600</xdr:colOff>
+      <xdr:colOff>327601</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Grafico 18"/>
+        <xdr:cNvPr id="5" name="Grafico 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6585120" y="6861960"/>
-        <a:ext cx="4527000" cy="2742480"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2439,19 +3404,25 @@
       <xdr:rowOff>26640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>334800</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>727523</xdr:colOff>
       <xdr:row>80</xdr:row>
       <xdr:rowOff>25920</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Grafico 19"/>
+        <xdr:cNvPr id="6" name="Grafico 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="626760" y="12051000"/>
-        <a:ext cx="4660200" cy="2742480"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2470,18 +3441,24 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>312120</xdr:colOff>
+      <xdr:colOff>312121</xdr:colOff>
       <xdr:row>79</xdr:row>
       <xdr:rowOff>178200</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Grafico 20"/>
+        <xdr:cNvPr id="7" name="Grafico 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6569640" y="12020400"/>
-        <a:ext cx="4527000" cy="2742480"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2491,346 +3468,796 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>23760</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>26640</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4543453" cy="2732541"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Grafico 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C166127-A3CC-40E8-931A-7FA3BAC6D02C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7560</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>178920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4421016" cy="2732541"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Grafico 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB446C4D-739E-4E0A-B171-18DFE1950D30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B2:N64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:N92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I47" activeCellId="0" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="99" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="9.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.44"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>100</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>200</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5">
         <v>400</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5">
         <v>800</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5">
         <v>1000</v>
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="n">
-        <v>0.09145</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>0.1059</v>
-      </c>
-      <c r="F6" s="3" t="n">
+      <c r="D6" s="3">
+        <v>9.1450000000000004E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.10589999999999999</v>
+      </c>
+      <c r="F6" s="3">
         <v>0.10865</v>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="G6" s="3">
         <v>0.11475</v>
       </c>
-      <c r="H6" s="3" t="n">
-        <v>0.11535</v>
-      </c>
-      <c r="I6" s="3" t="n">
-        <v>0.1165</v>
+      <c r="H6" s="3">
+        <v>0.11534999999999999</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.11650000000000001</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8">
         <v>1000</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8">
         <v>2000</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8">
         <v>4000</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8">
         <v>16000</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8">
         <v>32000</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D9" s="4">
         <v>66567.41</v>
       </c>
-      <c r="E9" s="4" t="n">
-        <v>88394.382</v>
-      </c>
-      <c r="F9" s="4" t="n">
-        <v>127427.437</v>
-      </c>
-      <c r="G9" s="4" t="n">
-        <v>454635.218</v>
-      </c>
-      <c r="H9" s="4" t="n">
-        <v>843234.062</v>
+      <c r="E9" s="4">
+        <v>88394.381999999998</v>
+      </c>
+      <c r="F9" s="4">
+        <v>127427.43700000001</v>
+      </c>
+      <c r="G9" s="4">
+        <v>454635.21799999999</v>
+      </c>
+      <c r="H9" s="4">
+        <v>843234.06200000003</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>0</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32">
         <v>100</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32">
         <v>200</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32">
         <v>400</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32">
         <v>800</v>
       </c>
-      <c r="I32" s="0" t="n">
+      <c r="I32">
         <v>1000</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="0" t="s">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="6" t="n">
+      <c r="D33" s="6">
         <v>10.507</v>
       </c>
-      <c r="E33" s="6" t="n">
-        <v>10.614</v>
-      </c>
-      <c r="F33" s="6" t="n">
+      <c r="E33" s="6">
+        <v>10.614000000000001</v>
+      </c>
+      <c r="F33" s="6">
         <v>10.5945</v>
       </c>
-      <c r="G33" s="6" t="n">
+      <c r="G33" s="6">
         <v>10.7027</v>
       </c>
-      <c r="H33" s="6" t="n">
+      <c r="H33" s="6">
         <v>10.7037</v>
       </c>
-      <c r="I33" s="6" t="n">
-        <v>10.8234</v>
+      <c r="I33" s="6">
+        <v>10.823399999999999</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="K34" s="5"/>
       <c r="M34" s="5"/>
     </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35">
         <v>1000</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35">
         <v>2000</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35">
         <v>4000</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35">
         <v>16000</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35">
         <v>32000</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="0" t="s">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="4" t="n">
+      <c r="D36" s="4">
         <v>737.39</v>
       </c>
-      <c r="E36" s="4" t="n">
+      <c r="E36" s="4">
         <v>1504.58</v>
       </c>
-      <c r="F36" s="4" t="n">
+      <c r="F36" s="4">
         <v>2999.09</v>
       </c>
-      <c r="G36" s="4" t="n">
-        <v>11512.933</v>
-      </c>
-      <c r="H36" s="4" t="n">
+      <c r="G36" s="4">
+        <v>11512.933000000001</v>
+      </c>
+      <c r="H36" s="4">
         <v>23858.7</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
       <c r="N43" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B58" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
         <v>2</v>
       </c>
-      <c r="D60" s="0" t="n">
+      <c r="D60">
         <v>1</v>
       </c>
-      <c r="E60" s="0" t="n">
+      <c r="E60">
         <v>100</v>
       </c>
-      <c r="F60" s="0" t="n">
+      <c r="F60">
         <v>200</v>
       </c>
-      <c r="G60" s="0" t="n">
+      <c r="G60">
         <v>400</v>
       </c>
-      <c r="H60" s="0" t="n">
+      <c r="H60">
         <v>800</v>
       </c>
-      <c r="I60" s="0" t="n">
+      <c r="I60">
         <v>1000</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="0" t="s">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
         <v>3</v>
       </c>
-      <c r="D61" s="6" t="n">
-        <v>50.664249</v>
-      </c>
-      <c r="E61" s="6" t="n">
-        <v>50.6443</v>
-      </c>
-      <c r="F61" s="6" t="n">
-        <v>50.7387</v>
-      </c>
-      <c r="G61" s="6" t="n">
-        <v>50.7908</v>
-      </c>
-      <c r="H61" s="6" t="n">
-        <v>50.7981</v>
-      </c>
-      <c r="I61" s="6" t="n">
+      <c r="D61" s="6">
+        <v>50.664248999999998</v>
+      </c>
+      <c r="E61" s="6">
+        <v>50.644300000000001</v>
+      </c>
+      <c r="F61" s="6">
+        <v>50.738700000000001</v>
+      </c>
+      <c r="G61" s="6">
+        <v>50.790799999999997</v>
+      </c>
+      <c r="H61" s="6">
+        <v>50.798099999999998</v>
+      </c>
+      <c r="I61" s="6">
         <v>50.9861</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0" t="s">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="0" t="n">
+      <c r="D63">
         <v>1000</v>
       </c>
-      <c r="E63" s="0" t="n">
+      <c r="E63">
         <v>2000</v>
       </c>
-      <c r="F63" s="0" t="n">
+      <c r="F63">
         <v>4000</v>
       </c>
-      <c r="G63" s="0" t="n">
+      <c r="G63">
         <v>16000</v>
       </c>
-      <c r="H63" s="0" t="n">
+      <c r="H63">
         <v>32000</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="0" t="s">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="4" t="n">
-        <v>157.98</v>
-      </c>
-      <c r="E64" s="4" t="n">
-        <v>312.8258</v>
-      </c>
-      <c r="F64" s="4" t="n">
+      <c r="D64" s="4">
+        <v>157.97999999999999</v>
+      </c>
+      <c r="E64" s="4">
+        <v>312.82580000000002</v>
+      </c>
+      <c r="F64" s="4">
         <v>620.9144</v>
       </c>
-      <c r="G64" s="4" t="n">
-        <v>2503.5878</v>
-      </c>
-      <c r="H64" s="4" t="n">
-        <v>5056.864</v>
+      <c r="G64" s="4">
+        <v>2503.5877999999998</v>
+      </c>
+      <c r="H64" s="4">
+        <v>5056.8639999999996</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B86" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>100</v>
+      </c>
+      <c r="F88">
+        <v>200</v>
+      </c>
+      <c r="G88">
+        <v>400</v>
+      </c>
+      <c r="H88">
+        <v>800</v>
+      </c>
+      <c r="I88">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="6">
+        <v>500.667419</v>
+      </c>
+      <c r="E89" s="6">
+        <v>500.67169200000001</v>
+      </c>
+      <c r="F89" s="6">
+        <v>500.66989999999998</v>
+      </c>
+      <c r="G89" s="6">
+        <v>500.72390000000001</v>
+      </c>
+      <c r="H89" s="6">
+        <v>500.87279999999998</v>
+      </c>
+      <c r="I89" s="6">
+        <v>500.91579999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91">
+        <v>1000</v>
+      </c>
+      <c r="E91">
+        <v>2000</v>
+      </c>
+      <c r="F91">
+        <v>4000</v>
+      </c>
+      <c r="G91">
+        <v>16000</v>
+      </c>
+      <c r="H91">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" s="4">
+        <v>16.0732</v>
+      </c>
+      <c r="E92" s="4">
+        <v>32.031199999999998</v>
+      </c>
+      <c r="F92" s="4">
+        <v>64.948999999999998</v>
+      </c>
+      <c r="G92" s="4">
+        <v>255.43940000000001</v>
+      </c>
+      <c r="H92" s="4">
+        <v>510.99</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ho risposto alle tue domande
</commit_message>
<xml_diff>
--- a/Assignment 3/Diagrams.xlsx
+++ b/Assignment 3/Diagrams.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alessandr.lombardin3\Desktop\assignment-di-reti\Assignment 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Desktop\assignment-di-reti\Assignment 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6538945B-8DD7-42E1-AB5A-3A439DA0E46C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -59,13 +60,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -89,6 +90,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -118,6 +132,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -236,7 +252,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -256,7 +271,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$C$6</c:f>
+              <c:f>Foglio1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -322,7 +337,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$D$5:$I$5</c:f>
+              <c:f>Foglio1!$B$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -349,7 +364,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$D$6:$I$6</c:f>
+              <c:f>Foglio1!$B$6:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -434,7 +449,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -520,7 +534,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -620,7 +633,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -640,7 +652,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$C$9</c:f>
+              <c:f>Foglio1!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -706,7 +718,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$D$8:$H$8</c:f>
+              <c:f>Foglio1!$B$26:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -730,7 +742,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$D$9:$H$9</c:f>
+              <c:f>Foglio1!$B$27:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -812,7 +824,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -916,7 +927,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1011,12 +1021,11 @@
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>RTT con delay di 10 ms</a:t>
+              <a:t>RTT con delay di 50 ms</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1036,7 +1045,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$C$33</c:f>
+              <c:f>Foglio1!$A$106</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1102,7 +1111,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$D$32:$I$32</c:f>
+              <c:f>Foglio1!$B$105:$G$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1129,794 +1138,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$D$33:$I$33</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.000000</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>10.507</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10.614000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.5945</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.7027</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.7037</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.823399999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8645-48E9-9B3A-9389F7C19815}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="59119462"/>
-        <c:axId val="71557302"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="59119462"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>PAYLOAD (Byte)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="71557302"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="71557302"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>RTT (Millisecondi)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="59119462"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>THROUGHPUT con delay di 10 ms</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Foglio1!$C$36</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>THPUT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="4472C4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4472C4"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Foglio1!$D$35:$H$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>32000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Foglio1!$D$36:$H$36</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>737.39</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1504.58</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2999.09</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11512.933000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>23858.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-212D-4BAD-8A0B-74651098D605}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="22102846"/>
-        <c:axId val="51360146"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="22102846"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>PAYLOAD (Byte)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="D9D9D9"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="51360146"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="51360146"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="D9D9D9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>THROUGHPUT (Kilobits</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t> per s</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="it-IT" sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="595959"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:rPr>
-                  <a:t>econdo)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="2.7910384021396308E-2"/>
-              <c:y val="0.16693847196674294"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="6480">
-            <a:noFill/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="22102846"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="D9D9D9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="it-IT" sz="1400" b="0" strike="noStrike" spc="-1">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>RTT con delay di 50 ms</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Foglio1!$C$61</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>RTT</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28440">
-              <a:solidFill>
-                <a:srgbClr val="4472C4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="4472C4"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Foglio1!$D$60:$I$60</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Foglio1!$D$61:$I$61</c:f>
+              <c:f>Foglio1!$B$106:$G$106</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.000000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2001,7 +1223,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2087,7 +1308,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2154,7 +1374,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -2187,7 +1407,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2207,7 +1426,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$C$64</c:f>
+              <c:f>Foglio1!$A$126</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2273,7 +1492,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$D$63:$H$63</c:f>
+              <c:f>Foglio1!$B$125:$F$125</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2297,7 +1516,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$D$64:$H$64</c:f>
+              <c:f>Foglio1!$B$126:$F$126</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2379,7 +1598,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2483,7 +1701,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2550,7 +1767,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -2590,7 +1807,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2610,7 +1826,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$C$89</c:f>
+              <c:f>Foglio1!$A$158</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2676,7 +1892,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$D$88:$I$88</c:f>
+              <c:f>Foglio1!$B$157:$G$157</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2703,7 +1919,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$D$89:$I$89</c:f>
+              <c:f>Foglio1!$B$158:$G$158</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.000000</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2788,7 +2004,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2874,7 +2089,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2941,7 +2155,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
@@ -2981,7 +2195,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3001,7 +2214,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Foglio1!$C$92</c:f>
+              <c:f>Foglio1!$A$180</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3067,7 +2280,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio1!$D$91:$H$91</c:f>
+              <c:f>Foglio1!$B$179:$F$179</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3091,7 +2304,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$D$92:$H$92</c:f>
+              <c:f>Foglio1!$B$180:$F$180</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3173,7 +2386,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3277,7 +2489,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3348,16 +2559,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>178560</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>142560</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>186261</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50194</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>209455</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>170973</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>49474</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3384,16 +2595,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>482760</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>197981</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>75582</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>340201</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>116997</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>65861</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3420,23 +2631,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>8280</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>354730</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>80519</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>712043</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>10800</xdr:rowOff>
+      <xdr:colOff>219523</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>79799</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Grafico 17">
+        <xdr:cNvPr id="6" name="Grafico 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3456,88 +2667,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>23040</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>327601</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Grafico 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>23760</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>423197</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>86557</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>727523</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Grafico 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>312121</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:colOff>142788</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>85837</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3556,7 +2695,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3564,10 +2703,10 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>23760</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>531760</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>134397</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4543453" cy="2732541"/>
     <xdr:graphicFrame macro="">
@@ -3589,7 +2728,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3597,10 +2736,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>178920</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>469379</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>55767</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4421016" cy="2732541"/>
     <xdr:graphicFrame macro="">
@@ -3622,7 +2761,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3927,431 +3066,435 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N92"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:N180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="99" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A179" sqref="A179:F180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" customWidth="1"/>
+    <col min="15" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="B5" s="7">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="C5" s="7">
         <v>100</v>
       </c>
-      <c r="F5">
+      <c r="D5" s="7">
         <v>200</v>
       </c>
-      <c r="G5">
+      <c r="E5" s="7">
         <v>400</v>
       </c>
-      <c r="H5">
+      <c r="F5" s="7">
         <v>800</v>
       </c>
-      <c r="I5">
+      <c r="G5" s="7">
         <v>1000</v>
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="3">
+        <v>9.1450000000000004E-2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.10589999999999999</v>
+      </c>
       <c r="D6" s="3">
-        <v>9.1450000000000004E-2</v>
+        <v>0.10865</v>
       </c>
       <c r="E6" s="3">
-        <v>0.10589999999999999</v>
+        <v>0.11475</v>
       </c>
       <c r="F6" s="3">
-        <v>0.10865</v>
+        <v>0.11534999999999999</v>
       </c>
       <c r="G6" s="3">
-        <v>0.11475</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.11534999999999999</v>
-      </c>
-      <c r="I6" s="3">
         <v>0.11650000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="B26" s="7">
         <v>1000</v>
       </c>
-      <c r="E8">
+      <c r="C26" s="7">
         <v>2000</v>
       </c>
-      <c r="F8">
+      <c r="D26" s="7">
         <v>4000</v>
       </c>
-      <c r="G8">
+      <c r="E26" s="7">
         <v>16000</v>
       </c>
-      <c r="H8">
+      <c r="F26" s="7">
         <v>32000</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="4">
+      <c r="B27" s="4">
         <v>66567.41</v>
       </c>
-      <c r="E9" s="4">
+      <c r="C27" s="4">
         <v>88394.381999999998</v>
       </c>
-      <c r="F9" s="4">
+      <c r="D27" s="4">
         <v>127427.43700000001</v>
       </c>
-      <c r="G9" s="4">
+      <c r="E27" s="4">
         <v>454635.21799999999</v>
       </c>
-      <c r="H9" s="4">
+      <c r="F27" s="4">
         <v>843234.06200000003</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K51" s="5"/>
+      <c r="M51" s="5"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
     </row>
-    <row r="30" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
+    <row r="54" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D32">
+      <c r="B57" s="7">
         <v>1</v>
       </c>
-      <c r="E32">
+      <c r="C57" s="7">
         <v>100</v>
       </c>
-      <c r="F32">
+      <c r="D57" s="7">
         <v>200</v>
       </c>
-      <c r="G32">
+      <c r="E57" s="7">
         <v>400</v>
       </c>
-      <c r="H32">
+      <c r="F57" s="7">
         <v>800</v>
       </c>
-      <c r="I32">
+      <c r="G57" s="7">
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="6">
+      <c r="B58" s="6">
         <v>10.507</v>
       </c>
-      <c r="E33" s="6">
+      <c r="C58" s="6">
         <v>10.614000000000001</v>
       </c>
-      <c r="F33" s="6">
+      <c r="D58" s="6">
         <v>10.5945</v>
       </c>
-      <c r="G33" s="6">
+      <c r="E58" s="6">
         <v>10.7027</v>
       </c>
-      <c r="H33" s="6">
+      <c r="F58" s="6">
         <v>10.7037</v>
       </c>
-      <c r="I33" s="6">
+      <c r="G58" s="6">
         <v>10.823399999999999</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K34" s="5"/>
-      <c r="M34" s="5"/>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D35">
+      <c r="B77" s="7">
         <v>1000</v>
       </c>
-      <c r="E35">
+      <c r="C77" s="7">
         <v>2000</v>
       </c>
-      <c r="F35">
+      <c r="D77" s="7">
         <v>4000</v>
       </c>
-      <c r="G35">
+      <c r="E77" s="7">
         <v>16000</v>
       </c>
-      <c r="H35">
+      <c r="F77" s="7">
         <v>32000</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="4">
+      <c r="B78" s="8">
         <v>737.39</v>
       </c>
-      <c r="E36" s="4">
+      <c r="C78" s="8">
         <v>1504.58</v>
       </c>
-      <c r="F36" s="4">
+      <c r="D78" s="8">
         <v>2999.09</v>
       </c>
-      <c r="G36" s="4">
+      <c r="E78" s="8">
         <v>11512.933000000001</v>
       </c>
-      <c r="H36" s="4">
+      <c r="F78" s="8">
         <v>23858.7</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
+    <row r="103" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="B103" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="7">
+        <v>1</v>
+      </c>
+      <c r="C105" s="7">
+        <v>100</v>
+      </c>
+      <c r="D105" s="7">
+        <v>200</v>
+      </c>
+      <c r="E105" s="7">
+        <v>400</v>
+      </c>
+      <c r="F105" s="7">
+        <v>800</v>
+      </c>
+      <c r="G105" s="7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106" s="6">
+        <v>50.664248999999998</v>
+      </c>
+      <c r="C106" s="6">
+        <v>50.644300000000001</v>
+      </c>
+      <c r="D106" s="6">
+        <v>50.738700000000001</v>
+      </c>
+      <c r="E106" s="6">
+        <v>50.790799999999997</v>
+      </c>
+      <c r="F106" s="6">
+        <v>50.798099999999998</v>
+      </c>
+      <c r="G106" s="6">
+        <v>50.9861</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B125" s="7">
+        <v>1000</v>
+      </c>
+      <c r="C125" s="7">
+        <v>2000</v>
+      </c>
+      <c r="D125" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E125" s="7">
+        <v>16000</v>
+      </c>
+      <c r="F125" s="7">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B126" s="4">
+        <v>157.97999999999999</v>
+      </c>
+      <c r="C126" s="4">
+        <v>312.82580000000002</v>
+      </c>
+      <c r="D126" s="4">
+        <v>620.9144</v>
+      </c>
+      <c r="E126" s="4">
+        <v>2503.5877999999998</v>
+      </c>
+      <c r="F126" s="4">
+        <v>5056.8639999999996</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B58" s="1" t="s">
-        <v>6</v>
+    <row r="155" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A157" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D60">
+      <c r="B157">
         <v>1</v>
       </c>
-      <c r="E60">
+      <c r="C157">
         <v>100</v>
       </c>
-      <c r="F60">
+      <c r="D157">
         <v>200</v>
       </c>
-      <c r="G60">
+      <c r="E157">
         <v>400</v>
       </c>
-      <c r="H60">
+      <c r="F157">
         <v>800</v>
       </c>
-      <c r="I60">
+      <c r="G157">
         <v>1000</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A158" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D61" s="6">
-        <v>50.664248999999998</v>
-      </c>
-      <c r="E61" s="6">
-        <v>50.644300000000001</v>
-      </c>
-      <c r="F61" s="6">
-        <v>50.738700000000001</v>
-      </c>
-      <c r="G61" s="6">
-        <v>50.790799999999997</v>
-      </c>
-      <c r="H61" s="6">
-        <v>50.798099999999998</v>
-      </c>
-      <c r="I61" s="6">
-        <v>50.9861</v>
+      <c r="B158" s="6">
+        <v>500.667419</v>
+      </c>
+      <c r="C158" s="6">
+        <v>500.67169200000001</v>
+      </c>
+      <c r="D158" s="6">
+        <v>500.66989999999998</v>
+      </c>
+      <c r="E158" s="6">
+        <v>500.72390000000001</v>
+      </c>
+      <c r="F158" s="6">
+        <v>500.87279999999998</v>
+      </c>
+      <c r="G158" s="6">
+        <v>500.91579999999999</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D63">
+      <c r="B179" s="7">
         <v>1000</v>
       </c>
-      <c r="E63">
+      <c r="C179" s="7">
         <v>2000</v>
       </c>
-      <c r="F63">
+      <c r="D179" s="7">
         <v>4000</v>
       </c>
-      <c r="G63">
+      <c r="E179" s="7">
         <v>16000</v>
       </c>
-      <c r="H63">
+      <c r="F179" s="7">
         <v>32000</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="4">
-        <v>157.97999999999999</v>
-      </c>
-      <c r="E64" s="4">
-        <v>312.82580000000002</v>
-      </c>
-      <c r="F64" s="4">
-        <v>620.9144</v>
-      </c>
-      <c r="G64" s="4">
-        <v>2503.5877999999998</v>
-      </c>
-      <c r="H64" s="4">
-        <v>5056.8639999999996</v>
-      </c>
-    </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B86" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>2</v>
-      </c>
-      <c r="D88">
-        <v>1</v>
-      </c>
-      <c r="E88">
-        <v>100</v>
-      </c>
-      <c r="F88">
-        <v>200</v>
-      </c>
-      <c r="G88">
-        <v>400</v>
-      </c>
-      <c r="H88">
-        <v>800</v>
-      </c>
-      <c r="I88">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
-        <v>3</v>
-      </c>
-      <c r="D89" s="6">
-        <v>500.667419</v>
-      </c>
-      <c r="E89" s="6">
-        <v>500.67169200000001</v>
-      </c>
-      <c r="F89" s="6">
-        <v>500.66989999999998</v>
-      </c>
-      <c r="G89" s="6">
-        <v>500.72390000000001</v>
-      </c>
-      <c r="H89" s="6">
-        <v>500.87279999999998</v>
-      </c>
-      <c r="I89" s="6">
-        <v>500.91579999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>2</v>
-      </c>
-      <c r="D91">
-        <v>1000</v>
-      </c>
-      <c r="E91">
-        <v>2000</v>
-      </c>
-      <c r="F91">
-        <v>4000</v>
-      </c>
-      <c r="G91">
-        <v>16000</v>
-      </c>
-      <c r="H91">
-        <v>32000</v>
-      </c>
-    </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C92" t="s">
-        <v>4</v>
-      </c>
-      <c r="D92" s="4">
+      <c r="B180" s="4">
         <v>16.0732</v>
       </c>
-      <c r="E92" s="4">
+      <c r="C180" s="4">
         <v>32.031199999999998</v>
       </c>
-      <c r="F92" s="4">
+      <c r="D180" s="4">
         <v>64.948999999999998</v>
       </c>
-      <c r="G92" s="4">
+      <c r="E180" s="4">
         <v>255.43940000000001</v>
       </c>
-      <c r="H92" s="4">
+      <c r="F180" s="4">
         <v>510.99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>